<commit_message>
Added Ca and its interactions with existing species
</commit_message>
<xml_diff>
--- a/pytzer/M88.xlsx
+++ b/pytzer/M88.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8850" windowHeight="6195" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8850" windowHeight="6195" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="b0" sheetId="1" r:id="rId1"/>
     <sheet name="b1" sheetId="2" r:id="rId2"/>
     <sheet name="Cphi" sheetId="3" r:id="rId3"/>
     <sheet name="theta" sheetId="4" r:id="rId4"/>
+    <sheet name="psi" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="18">
   <si>
     <t>cation</t>
   </si>
@@ -75,6 +76,12 @@
   </si>
   <si>
     <t>ion1</t>
+  </si>
+  <si>
+    <t>xion</t>
+  </si>
+  <si>
+    <t>Ca</t>
   </si>
 </sst>
 </file>
@@ -393,9 +400,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -492,6 +501,38 @@
         <v>0</v>
       </c>
       <c r="J3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1">
+        <v>-94.189583200000001</v>
+      </c>
+      <c r="D4" s="1">
+        <v>-4.0475002599999997E-2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2345.5036799999998</v>
+      </c>
+      <c r="F4" s="1">
+        <v>17.091229999999999</v>
+      </c>
+      <c r="G4" s="1">
+        <v>-0.92288584100000004</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1.5148812200000001E-5</v>
+      </c>
+      <c r="I4" s="1">
+        <v>-1.3908199999999999</v>
+      </c>
+      <c r="J4" s="1">
         <v>0</v>
       </c>
     </row>
@@ -502,10 +543,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,6 +653,41 @@
         <v>-5.9457814000000004</v>
       </c>
       <c r="K3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3.4786999999999999</v>
+      </c>
+      <c r="D4" s="1">
+        <v>-1.5417E-2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>3.1791000000000001E-5</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
         <v>2</v>
       </c>
     </row>
@@ -622,10 +698,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:J1"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,6 +799,38 @@
         <v>0</v>
       </c>
       <c r="J3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1">
+        <v>19.305602400000001</v>
+      </c>
+      <c r="D4" s="1">
+        <v>9.77090932E-3</v>
+      </c>
+      <c r="E4" s="1">
+        <v>-428.38374800000003</v>
+      </c>
+      <c r="F4" s="1">
+        <v>-3.5799634299999998</v>
+      </c>
+      <c r="G4" s="1">
+        <v>8.8206853799999999E-2</v>
+      </c>
+      <c r="H4" s="1">
+        <v>-4.6227023800000004E-6</v>
+      </c>
+      <c r="I4" s="1">
+        <v>9.9111346499999993</v>
+      </c>
+      <c r="J4" s="1">
         <v>0</v>
       </c>
     </row>
@@ -733,10 +841,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,6 +913,223 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.11559999999999999</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1.34211308E-2</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>-5.1021291700000004</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1">
+        <v>-3.0000000000000001E-3</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1">
+        <v>4.7627897699999998E-2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>-27.077050700000001</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>